<commit_message>
created mockapi, added utility.js to deal with custom objects, updated reports and notes
</commit_message>
<xml_diff>
--- a/other/Project_TimeLine_2021_1_Apr.xlsx
+++ b/other/Project_TimeLine_2021_1_Apr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\aztech-lms\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288B5183-1EA0-42B9-BABD-E909B16F621F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D05D24B-66FF-4340-B1FC-BCF88960E801}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>S/N</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Front-end: Dashboard main page</t>
   </si>
   <si>
-    <t>Implement existing pages first as discussed with Sanjay</t>
-  </si>
-  <si>
     <t>Front-end: Config</t>
   </si>
   <si>
@@ -141,7 +138,14 @@
     <t>Code refactoring</t>
   </si>
   <si>
-    <t>Will have reorganise how data is handled by the individual cards on the dashboard page</t>
+    <t>Front-end: Dashboard view data management</t>
+  </si>
+  <si>
+    <t>By moving data out of the individual card components, potentially less API calls will be required</t>
+  </si>
+  <si>
+    <t>Work on this at least till new pages or content added to Adobe XD link
+Expected to take a long time as it was originally not written in React, and I foresee some issues arising from that</t>
   </si>
 </sst>
 </file>
@@ -524,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0DE7D-B314-4018-AC47-8A93F1174983}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,7 +832,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -876,7 +880,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -900,7 +904,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -924,7 +928,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -947,7 +951,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -970,7 +974,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -989,32 +993,55 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" s="3">
         <v>44285</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="3">
+        <v>44287</v>
+      </c>
+      <c r="G20" s="3">
+        <v>44287</v>
+      </c>
       <c r="I20" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+    <row r="21" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21" s="3">
+        <v>44291</v>
+      </c>
+      <c r="F21" s="3">
+        <v>44300</v>
+      </c>
       <c r="H21" s="4"/>
+      <c r="I21" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -1026,7 +1053,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="I26" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1043,17 +1070,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="H28" t="s">
-        <v>27</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>